<commit_message>
Yellow highlighted validated cells
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C75D184-6C96-254A-9D50-A99CD8F3C5ED}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D961F0-5B1C-EA4A-8A42-3C09780510F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
@@ -243,12 +243,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -278,11 +284,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,8 +641,9 @@
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2">
-        <v>38</v>
+      <c r="C2" s="4">
+        <f>(44.9 + 40.3) / 2</f>
+        <v>42.599999999999994</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -676,8 +684,8 @@
       <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="C5">
-        <v>42.6</v>
+      <c r="C5" s="4">
+        <v>46</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -749,8 +757,8 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10">
-        <v>5.96</v>
+      <c r="C10" s="4">
+        <v>4.76</v>
       </c>
       <c r="D10" t="s">
         <v>12</v>
@@ -763,8 +771,8 @@
       <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="C11">
-        <v>1.49</v>
+      <c r="C11" s="4">
+        <v>4.28</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -791,7 +799,7 @@
       <c r="B13" t="s">
         <v>32</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="4">
         <v>4.5199999999999996</v>
       </c>
       <c r="D13" t="s">
@@ -805,8 +813,8 @@
       <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C14">
-        <v>1.2</v>
+      <c r="C14" s="4">
+        <v>1.8</v>
       </c>
       <c r="D14" t="s">
         <v>35</v>
@@ -822,7 +830,7 @@
       <c r="B15" t="s">
         <v>37</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="4">
         <v>3.62</v>
       </c>
       <c r="D15" t="s">
@@ -836,7 +844,7 @@
       <c r="B16" t="s">
         <v>38</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="4">
         <v>1.45</v>
       </c>
       <c r="D16" t="s">
@@ -864,7 +872,7 @@
       <c r="B18" t="s">
         <v>40</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="4">
         <v>2.54</v>
       </c>
       <c r="D18" t="s">
@@ -878,8 +886,8 @@
       <c r="B19" t="s">
         <v>41</v>
       </c>
-      <c r="C19">
-        <v>4</v>
+      <c r="C19" s="4">
+        <v>5</v>
       </c>
       <c r="D19" t="s">
         <v>35</v>
@@ -923,7 +931,7 @@
       <c r="B22" t="s">
         <v>45</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="4">
         <v>4.8499999999999996</v>
       </c>
       <c r="D22" t="s">
@@ -937,8 +945,8 @@
       <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C23">
-        <v>4</v>
+      <c r="C23" s="4">
+        <v>7.5</v>
       </c>
       <c r="D23" t="s">
         <v>35</v>
@@ -951,8 +959,9 @@
       <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="C24">
-        <v>25</v>
+      <c r="C24" s="4">
+        <f>46*0.48</f>
+        <v>22.08</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -993,8 +1002,8 @@
       <c r="B27" t="s">
         <v>51</v>
       </c>
-      <c r="C27">
-        <v>78500</v>
+      <c r="C27" s="4">
+        <v>78400</v>
       </c>
       <c r="D27" t="s">
         <v>42</v>
@@ -1010,8 +1019,8 @@
       <c r="B28" t="s">
         <v>61</v>
       </c>
-      <c r="C28">
-        <v>19.3</v>
+      <c r="C28" s="4">
+        <v>22.21</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
isolated variables to excel sheet
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D961F0-5B1C-EA4A-8A42-3C09780510F1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6069F3CA-B1AC-4F4D-9E33-EE4AD8AA10DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="README" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
   <si>
     <t>Instructions:</t>
   </si>
@@ -220,6 +220,45 @@
   </si>
   <si>
     <t>Distance of main gears from nose</t>
+  </si>
+  <si>
+    <t>rootChordLen_w</t>
+  </si>
+  <si>
+    <t>Root chord Length</t>
+  </si>
+  <si>
+    <t>tipChordLen_w</t>
+  </si>
+  <si>
+    <t>Tip chord Length</t>
+  </si>
+  <si>
+    <t>wingSemiSpan</t>
+  </si>
+  <si>
+    <t>Semi span of main wing</t>
+  </si>
+  <si>
+    <t>fuelTankLen</t>
+  </si>
+  <si>
+    <t>Pct of main wing semi-span</t>
+  </si>
+  <si>
+    <t>engineLoc_1</t>
+  </si>
+  <si>
+    <t>engineLoc_2</t>
+  </si>
+  <si>
+    <t>Length of engine from root of wing</t>
+  </si>
+  <si>
+    <t>engineWeight</t>
+  </si>
+  <si>
+    <t>Weight of engine</t>
   </si>
 </sst>
 </file>
@@ -284,12 +323,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -989,7 +1029,7 @@
         <v>49</v>
       </c>
       <c r="C26">
-        <v>1.1000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
@@ -1013,19 +1053,118 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="4">
+        <v>8.1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="4">
+        <v>1.62</v>
+      </c>
+      <c r="D29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="4">
+        <f>36.41/2</f>
+        <v>18.204999999999998</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" s="4">
+        <v>7.0750000000000002</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="4">
+        <v>11.875</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>74</v>
+      </c>
+      <c r="C34" s="4">
+        <v>2177</v>
+      </c>
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>60</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B35" t="s">
         <v>61</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C35" s="4">
         <v>22.21</v>
       </c>
-      <c r="D28" t="s">
-        <v>12</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>

<commit_message>
renamed ac_w to x_ac
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6069F3CA-B1AC-4F4D-9E33-EE4AD8AA10DA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1526D112-6514-7A49-ABBF-39723BD5C143}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
@@ -177,9 +177,6 @@
     <t>x_cg</t>
   </si>
   <si>
-    <t>ac_w</t>
-  </si>
-  <si>
     <t>CM0_w</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>Take-off weight of aircraft</t>
   </si>
   <si>
-    <t>Aerodynamic center from wing</t>
-  </si>
-  <si>
     <t>Distance of center of gravity from nose</t>
   </si>
   <si>
@@ -259,6 +253,12 @@
   </si>
   <si>
     <t>Weight of engine</t>
+  </si>
+  <si>
+    <t>Aerodynamic center from nose</t>
+  </si>
+  <si>
+    <t>x_ac</t>
   </si>
 </sst>
 </file>
@@ -647,7 +647,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -694,7 +694,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C3">
         <v>15</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C4">
         <v>18</v>
@@ -938,7 +938,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C20" s="3">
         <v>15300</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C21">
         <v>1.1000000000000001</v>
@@ -1007,12 +1007,12 @@
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C25">
         <v>19</v>
@@ -1021,12 +1021,12 @@
         <v>12</v>
       </c>
       <c r="E25" t="s">
-        <v>53</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26">
         <v>-0.08</v>
@@ -1040,7 +1040,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C27" s="4">
         <v>78400</v>
@@ -1049,12 +1049,12 @@
         <v>42</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28" s="4">
         <v>8.1</v>
@@ -1063,12 +1063,12 @@
         <v>12</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29" s="4">
         <v>1.62</v>
@@ -1077,12 +1077,12 @@
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30" s="4">
         <f>36.41/2</f>
@@ -1092,12 +1092,12 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31" s="5">
         <v>0.8</v>
@@ -1106,12 +1106,12 @@
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32" s="4">
         <v>7.0750000000000002</v>
@@ -1120,12 +1120,12 @@
         <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C33" s="4">
         <v>11.875</v>
@@ -1134,12 +1134,12 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C34" s="4">
         <v>2177</v>
@@ -1148,15 +1148,15 @@
         <v>42</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B35" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C35" s="4">
         <v>22.21</v>
@@ -1165,7 +1165,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1196,12 +1196,12 @@
     </row>
     <row r="4" spans="1:1" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Bug fixes for logical errors
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899FD3C3-C57D-0C42-A26E-D836ADC9A31A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E20B28E-2377-B542-A1EA-344CBD1255C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,7 +955,7 @@
         <v>49</v>
       </c>
       <c r="C21">
-        <v>1.1000000000000001</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Revised and prettified graphs
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E20B28E-2377-B542-A1EA-344CBD1255C6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2512D557-309A-3646-A281-0FAB95821132}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="79">
   <si>
     <t>Instructions:</t>
   </si>
@@ -259,6 +259,15 @@
   </si>
   <si>
     <t>x_ac</t>
+  </si>
+  <si>
+    <t>Aerodynamic center from datum [z]</t>
+  </si>
+  <si>
+    <t>z_h</t>
+  </si>
+  <si>
+    <t>Measured from datum [z]</t>
   </si>
 </sst>
 </file>
@@ -644,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -826,13 +835,13 @@
         <v>30</v>
       </c>
       <c r="C12">
-        <v>1</v>
+        <v>3.28</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -965,170 +974,170 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C22" s="4">
+        <v>8.65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C23" s="4">
         <v>4.8499999999999996</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="4">
-        <v>7.5</v>
-      </c>
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="E23" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="4">
+        <v>7.5</v>
+      </c>
+      <c r="D24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="4">
+      <c r="C25" s="4">
         <f>46*0.48</f>
         <v>22.08</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25">
-        <v>21.5</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>48</v>
+        <v>75</v>
       </c>
       <c r="C26">
-        <v>-0.08</v>
+        <v>21.5</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="E26" t="s">
-        <v>44</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="4">
-        <v>78400</v>
+        <v>48</v>
+      </c>
+      <c r="C27">
+        <v>-0.08</v>
       </c>
       <c r="D27" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C28" s="4">
-        <v>8.1</v>
+        <v>78400</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="E28" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4">
-        <v>1.62</v>
+        <v>8.1</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="4">
+        <v>1.62</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>65</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <f>36.41/2</f>
         <v>18.204999999999998</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="5">
-        <v>0.8</v>
-      </c>
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E31" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="4">
-        <v>7.0750000000000002</v>
+        <v>67</v>
+      </c>
+      <c r="C32" s="5">
+        <v>0.8</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C33" s="4">
-        <v>11.875</v>
+        <v>7.0750000000000002</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -1139,32 +1148,46 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="4">
+        <v>11.875</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C35" s="4">
         <v>2177</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>42</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E35" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>58</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C36" s="4">
         <v>22.21</v>
       </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed wing_1 torque and fuselage_3 bm
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16AF89D-A04C-3C4C-8641-A3EC687D5900}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF59EE-E2D0-404E-B517-AEF758D3F326}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
+    <workbookView xWindow="4040" yWindow="720" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -664,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1061,7 +1061,7 @@
         <v>75</v>
       </c>
       <c r="C27">
-        <v>21.5</v>
+        <v>24.7</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Fixed horizontal_stabilizer cases, vs is correct
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAF59EE-E2D0-404E-B517-AEF758D3F326}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C5B127-D99E-F648-B4C7-702766CFA84E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="720" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
+    <workbookView xWindow="4040" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -664,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
minor modifications -- unsure if all correct
</commit_message>
<xml_diff>
--- a/geometryVariables.xlsx
+++ b/geometryVariables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geraldlow/twistInfidel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\icnas3.cc.ic.ac.uk\bcl15\Desktop\twistInfidel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C5B127-D99E-F648-B4C7-702766CFA84E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CD6DE7-BACC-40AA-9D03-56A00FFBE600}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="460" windowWidth="12800" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
+    <workbookView xWindow="4035" yWindow="465" windowWidth="12795" windowHeight="14580" xr2:uid="{1CCC08A1-6F62-9442-832C-C6AF866E95D9}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
   <si>
     <t>Instructions:</t>
   </si>
@@ -277,6 +277,12 @@
   </si>
   <si>
     <t>Take-off angle of attack</t>
+  </si>
+  <si>
+    <t>Distance of leading edge of wing from nose</t>
+  </si>
+  <si>
+    <t>x_le_w</t>
   </si>
 </sst>
 </file>
@@ -341,13 +347,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,20 +667,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D1DC7C-7FC1-054D-A5A3-14F3A3C04097}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -692,7 +697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -710,12 +715,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>55</v>
       </c>
-      <c r="C3">
-        <v>15</v>
+      <c r="C3" s="4">
+        <v>20.2</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -724,12 +729,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>56</v>
       </c>
-      <c r="C4">
-        <v>18</v>
+      <c r="C4" s="4">
+        <v>24.3</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -738,7 +743,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>15</v>
       </c>
@@ -752,7 +757,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>17</v>
       </c>
@@ -766,7 +771,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>19</v>
       </c>
@@ -780,7 +785,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>22</v>
       </c>
@@ -794,12 +799,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>24</v>
       </c>
       <c r="C9">
-        <v>18</v>
+        <v>24.3</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -808,7 +813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>79</v>
       </c>
@@ -822,7 +827,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -839,7 +844,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -853,7 +858,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>30</v>
       </c>
@@ -867,7 +872,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>32</v>
       </c>
@@ -881,7 +886,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>34</v>
       </c>
@@ -895,7 +900,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -912,7 +917,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>38</v>
       </c>
@@ -926,7 +931,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -940,7 +945,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>40</v>
       </c>
@@ -954,7 +959,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>41</v>
       </c>
@@ -968,7 +973,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>57</v>
       </c>
@@ -982,7 +987,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>49</v>
       </c>
@@ -996,7 +1001,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>77</v>
       </c>
@@ -1010,7 +1015,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1032,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>46</v>
       </c>
@@ -1041,7 +1046,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>47</v>
       </c>
@@ -1056,125 +1061,125 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="4">
+        <v>19</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>75</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>24.7</v>
       </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C28">
+      <c r="C29" s="4">
         <v>-0.08</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D29" t="s">
         <v>35</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E29" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C30" s="4">
         <v>78400</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D30" t="s">
         <v>42</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E30" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>61</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C31" s="4">
         <v>8.1</v>
       </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C32" s="4">
         <v>1.62</v>
       </c>
-      <c r="D31" t="s">
-        <v>12</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>65</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C33" s="4">
         <f>36.41/2</f>
         <v>18.204999999999998</v>
       </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C34" s="4">
         <v>0.8</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D34" t="s">
         <v>35</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E34" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C35" s="4">
         <v>7.0750000000000002</v>
-      </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>70</v>
-      </c>
-      <c r="C35" s="4">
-        <v>11.875</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -1183,34 +1188,48 @@
         <v>71</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="4">
+        <v>11.875</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C37" s="4">
         <v>2177</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>42</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>59</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C38" s="4">
         <v>22.21</v>
       </c>
-      <c r="D37" t="s">
-        <v>12</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D38" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1227,30 +1246,30 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
     </row>
   </sheetData>

</xml_diff>